<commit_message>
Update: Reformat power consumption summary
</commit_message>
<xml_diff>
--- a/Documents/PowerConsumption/Summary.xlsx
+++ b/Documents/PowerConsumption/Summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Workspace\KLTN-WeatherForecast\Documents\PowerConsumption\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94964BFF-9E92-4231-A531-21B8B3840D0C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98CAB9AC-173D-4D9A-8AE3-B9113A72D345}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{23813ABA-6C47-4AC0-8297-3CD24E81FA7D}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>Voltage</t>
   </si>
@@ -39,20 +39,32 @@
     <t>Power</t>
   </si>
   <si>
-    <t>Mili Ampere</t>
-  </si>
-  <si>
     <t>Version</t>
   </si>
   <si>
-    <t>3 with Charge</t>
+    <t>Atmega</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>STM8</t>
+  </si>
+  <si>
+    <t>Charging</t>
+  </si>
+  <si>
+    <t>Current</t>
+  </si>
+  <si>
+    <t>Sleep modules</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,22 +74,35 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -85,16 +110,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,107 +454,121 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E81A7E71-FE4B-4DFC-ACF0-BE163F34F7C2}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18:G18"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.125" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
-    <col min="3" max="3" width="18.125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="1" max="1" width="8.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
         <v>2016</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>5</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>23.4</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <f>B2*C2</f>
         <v>117</v>
       </c>
+      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>17.3</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="2">
         <f>B3*C3</f>
         <v>86.5</v>
       </c>
+      <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
         <v>3.3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>9.3000000000000007</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="2">
         <f t="shared" ref="D4:D6" si="0">B4*C4</f>
         <v>30.69</v>
       </c>
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>11.5</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="2">
         <f t="shared" si="0"/>
         <v>103.5</v>
       </c>
+      <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
         <v>9</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>250</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <f t="shared" si="0"/>
         <v>2250</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>